<commit_message>
fix: regenerate batch template with clinical fields
Template was stale - regenerated to include PainWorst, PainBest,
PainCurrent, SymptomDuration, PainRadiation, PainTypes, and other
clinical columns required by the updated parser.

Generated with [Claude Code](https://claude.ai/code)
via [Happy](https://happy.engineering)

Co-Authored-By: Claude <noreply@anthropic.com>
Co-Authored-By: Happy <yesreply@happy.engineering>
</commit_message>
<xml_diff>
--- a/templates/batch-template.xlsx
+++ b/templates/batch-template.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <workbookPr codeName="ThisWorkbook"/>
   <sheets>
-    <sheet name="Batch" sheetId="1" r:id="rId1"/>
+    <sheet name="Patients" sheetId="1" r:id="rId1"/>
     <sheet name="Instructions" sheetId="2" r:id="rId2"/>
   </sheets>
 </workbook>
@@ -398,287 +398,313 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K7"/>
+  <dimension ref="A1:U4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <cols>
-    <col min="1" max="1" width="6.83203125" customWidth="1"/>
-    <col min="2" max="2" width="30.83203125" customWidth="1"/>
-    <col min="3" max="3" width="8.83203125" customWidth="1"/>
-    <col min="4" max="4" width="12.83203125" customWidth="1"/>
-    <col min="5" max="5" width="14.83203125" customWidth="1"/>
-    <col min="6" max="6" width="12.83203125" customWidth="1"/>
-    <col min="7" max="7" width="10.83203125" customWidth="1"/>
-    <col min="8" max="8" width="20.83203125" customWidth="1"/>
-    <col min="9" max="9" width="20.83203125" customWidth="1"/>
-    <col min="10" max="10" width="20.83203125" customWidth="1"/>
-    <col min="11" max="11" width="20.83203125" customWidth="1"/>
+    <col min="1" max="1" width="30.83203125" customWidth="1"/>
+    <col min="2" max="2" width="8.83203125" customWidth="1"/>
+    <col min="3" max="3" width="12.83203125" customWidth="1"/>
+    <col min="4" max="4" width="14.83203125" customWidth="1"/>
+    <col min="5" max="5" width="12.83203125" customWidth="1"/>
+    <col min="6" max="6" width="20.83203125" customWidth="1"/>
+    <col min="7" max="7" width="20.83203125" customWidth="1"/>
+    <col min="8" max="8" width="12.83203125" customWidth="1"/>
+    <col min="9" max="9" width="10.83203125" customWidth="1"/>
+    <col min="10" max="10" width="10.83203125" customWidth="1"/>
+    <col min="11" max="11" width="12.83203125" customWidth="1"/>
+    <col min="12" max="12" width="16.83203125" customWidth="1"/>
+    <col min="13" max="13" width="25.83203125" customWidth="1"/>
+    <col min="14" max="14" width="20.83203125" customWidth="1"/>
+    <col min="15" max="15" width="20.83203125" customWidth="1"/>
+    <col min="16" max="16" width="35.83203125" customWidth="1"/>
+    <col min="17" max="17" width="35.83203125" customWidth="1"/>
+    <col min="18" max="18" width="12.83203125" customWidth="1"/>
+    <col min="19" max="19" width="14.83203125" customWidth="1"/>
+    <col min="20" max="20" width="20.83203125" customWidth="1"/>
+    <col min="21" max="21" width="25.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" t="str">
-        <v>DOS</v>
+        <v>Patient</v>
       </c>
       <c r="B1" t="str">
-        <v>Patient</v>
+        <v>Gender</v>
       </c>
       <c r="C1" t="str">
-        <v>Gender</v>
+        <v>Insurance</v>
       </c>
       <c r="D1" t="str">
-        <v>Insurance</v>
+        <v>BodyPart</v>
       </c>
       <c r="E1" t="str">
-        <v>BodyPart</v>
+        <v>Laterality</v>
       </c>
       <c r="F1" t="str">
-        <v>Laterality</v>
+        <v>ICD</v>
       </c>
       <c r="G1" t="str">
-        <v>NoteType</v>
+        <v>CPT</v>
       </c>
       <c r="H1" t="str">
-        <v>ICD</v>
+        <v>TotalVisits</v>
       </c>
       <c r="I1" t="str">
-        <v>CPT</v>
+        <v>PainWorst</v>
       </c>
       <c r="J1" t="str">
+        <v>PainBest</v>
+      </c>
+      <c r="K1" t="str">
+        <v>PainCurrent</v>
+      </c>
+      <c r="L1" t="str">
+        <v>SymptomDuration</v>
+      </c>
+      <c r="M1" t="str">
+        <v>PainRadiation</v>
+      </c>
+      <c r="N1" t="str">
+        <v>PainTypes</v>
+      </c>
+      <c r="O1" t="str">
+        <v>AssociatedSymptoms</v>
+      </c>
+      <c r="P1" t="str">
+        <v>CausativeFactors</v>
+      </c>
+      <c r="Q1" t="str">
+        <v>RelievingFactors</v>
+      </c>
+      <c r="R1" t="str">
+        <v>SymptomScale</v>
+      </c>
+      <c r="S1" t="str">
+        <v>PainFrequency</v>
+      </c>
+      <c r="T1" t="str">
         <v>SecondaryParts</v>
       </c>
-      <c r="K1" t="str">
+      <c r="U1" t="str">
         <v>History</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2">
-        <v>1</v>
+      <c r="A2" t="str">
+        <v>CHEN,AIJIN(09/27/1956)</v>
       </c>
       <c r="B2" t="str">
-        <v>CHEN,AIJIN(09/27/1956)</v>
+        <v>F</v>
       </c>
       <c r="C2" t="str">
+        <v>HF</v>
+      </c>
+      <c r="D2" t="str">
+        <v>LBP</v>
+      </c>
+      <c r="E2" t="str">
+        <v>B</v>
+      </c>
+      <c r="F2" t="str">
+        <v>M54.50,M54.41</v>
+      </c>
+      <c r="G2" t="str">
+        <v>97810,97811x3</v>
+      </c>
+      <c r="H2">
+        <v>12</v>
+      </c>
+      <c r="I2">
+        <v>8</v>
+      </c>
+      <c r="J2">
+        <v>3</v>
+      </c>
+      <c r="K2">
+        <v>6</v>
+      </c>
+      <c r="L2" t="str">
+        <v>3 year(s)</v>
+      </c>
+      <c r="M2" t="str">
+        <v>without radiation</v>
+      </c>
+      <c r="N2" t="str">
+        <v>Dull,Aching</v>
+      </c>
+      <c r="O2" t="str">
+        <v>soreness</v>
+      </c>
+      <c r="P2" t="str">
+        <v>age related/degenerative changes</v>
+      </c>
+      <c r="Q2" t="str">
+        <v>Changing positions,Resting,Massage</v>
+      </c>
+      <c r="R2" t="str">
+        <v>70%-80%</v>
+      </c>
+      <c r="S2" t="str">
+        <v>Constant</v>
+      </c>
+      <c r="T2" t="str">
+        <v/>
+      </c>
+      <c r="U2" t="str">
+        <v>Hypertension</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="str">
+        <v>WANG,MEI(03/15/1960)</v>
+      </c>
+      <c r="B3" t="str">
         <v>F</v>
       </c>
-      <c r="D2" t="str">
-        <v>HF</v>
-      </c>
-      <c r="E2" t="str">
-        <v>LBP</v>
-      </c>
-      <c r="F2" t="str">
-        <v>B</v>
-      </c>
-      <c r="G2" t="str">
-        <v>IE</v>
-      </c>
-      <c r="H2" t="str">
-        <v>M54.50,M54.41</v>
-      </c>
-      <c r="I2" t="str">
-        <v>97810,97811x3</v>
-      </c>
-      <c r="J2" t="str">
+      <c r="C3" t="str">
+        <v>WC</v>
+      </c>
+      <c r="D3" t="str">
+        <v>SHOULDER</v>
+      </c>
+      <c r="E3" t="str">
+        <v>R</v>
+      </c>
+      <c r="F3" t="str">
+        <v>M75.11,M25.511</v>
+      </c>
+      <c r="G3" t="str">
         <v/>
       </c>
-      <c r="K2" t="str">
+      <c r="H3">
+        <v>8</v>
+      </c>
+      <c r="I3">
+        <v>7</v>
+      </c>
+      <c r="J3">
+        <v>2</v>
+      </c>
+      <c r="K3">
+        <v>5</v>
+      </c>
+      <c r="L3" t="str">
+        <v>6 month(s)</v>
+      </c>
+      <c r="M3" t="str">
+        <v>with radiation to R arm</v>
+      </c>
+      <c r="N3" t="str">
+        <v>Dull,Stabbing</v>
+      </c>
+      <c r="O3" t="str">
+        <v>stiffness,soreness</v>
+      </c>
+      <c r="P3" t="str">
+        <v>over used due to heavy household chores</v>
+      </c>
+      <c r="Q3" t="str">
+        <v>Resting,Applying heating pad</v>
+      </c>
+      <c r="R3" t="str">
+        <v>60%-70%</v>
+      </c>
+      <c r="S3" t="str">
+        <v>Frequent</v>
+      </c>
+      <c r="T3" t="str">
+        <v>NECK</v>
+      </c>
+      <c r="U3" t="str">
+        <v>Diabetes,Osteoporosis</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="str">
+        <v>LI,HONG(11/20/1965)</v>
+      </c>
+      <c r="B4" t="str">
+        <v>M</v>
+      </c>
+      <c r="C4" t="str">
+        <v>OPTUM</v>
+      </c>
+      <c r="D4" t="str">
+        <v>KNEE</v>
+      </c>
+      <c r="E4" t="str">
+        <v>L</v>
+      </c>
+      <c r="F4" t="str">
+        <v>M25.562,M17.12</v>
+      </c>
+      <c r="G4" t="str">
         <v/>
       </c>
-    </row>
-    <row r="3">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3" t="str">
-        <v>CHEN,AIJIN(09/27/1956)</v>
-      </c>
-      <c r="C3" t="str">
-        <v>F</v>
-      </c>
-      <c r="D3" t="str">
-        <v>HF</v>
-      </c>
-      <c r="E3" t="str">
-        <v>LBP</v>
-      </c>
-      <c r="F3" t="str">
-        <v>B</v>
-      </c>
-      <c r="G3" t="str">
-        <v>TX</v>
-      </c>
-      <c r="H3" t="str">
+      <c r="H4">
+        <v>10</v>
+      </c>
+      <c r="I4">
+        <v>9</v>
+      </c>
+      <c r="J4">
+        <v>4</v>
+      </c>
+      <c r="K4">
+        <v>7</v>
+      </c>
+      <c r="L4" t="str">
+        <v>many year(s)</v>
+      </c>
+      <c r="M4" t="str">
+        <v>without radiation</v>
+      </c>
+      <c r="N4" t="str">
+        <v>Aching,Stabbing</v>
+      </c>
+      <c r="O4" t="str">
+        <v>weakness,stiffness</v>
+      </c>
+      <c r="P4" t="str">
+        <v>age related/degenerative changes,prolong walking</v>
+      </c>
+      <c r="Q4" t="str">
+        <v>Resting,Massage,Medications</v>
+      </c>
+      <c r="R4" t="str">
+        <v>80%-90%</v>
+      </c>
+      <c r="S4" t="str">
+        <v>Constant</v>
+      </c>
+      <c r="T4" t="str">
         <v/>
       </c>
-      <c r="I3" t="str">
-        <v/>
-      </c>
-      <c r="J3" t="str">
-        <v/>
-      </c>
-      <c r="K3" t="str">
-        <v/>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4" t="str">
-        <v>CHEN,AIJIN(09/27/1956)</v>
-      </c>
-      <c r="C4" t="str">
-        <v>F</v>
-      </c>
-      <c r="D4" t="str">
-        <v>HF</v>
-      </c>
-      <c r="E4" t="str">
-        <v>LBP</v>
-      </c>
-      <c r="F4" t="str">
-        <v>B</v>
-      </c>
-      <c r="G4" t="str">
-        <v>TX</v>
-      </c>
-      <c r="H4" t="str">
-        <v/>
-      </c>
-      <c r="I4" t="str">
-        <v/>
-      </c>
-      <c r="J4" t="str">
-        <v/>
-      </c>
-      <c r="K4" t="str">
-        <v/>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5" t="str">
-        <v>CHEN,AIJIN(09/27/1956)</v>
-      </c>
-      <c r="C5" t="str">
-        <v>F</v>
-      </c>
-      <c r="D5" t="str">
-        <v>HF</v>
-      </c>
-      <c r="E5" t="str">
-        <v>LBP</v>
-      </c>
-      <c r="F5" t="str">
-        <v>B</v>
-      </c>
-      <c r="G5" t="str">
-        <v>RE</v>
-      </c>
-      <c r="H5" t="str">
-        <v/>
-      </c>
-      <c r="I5" t="str">
-        <v>97161</v>
-      </c>
-      <c r="J5" t="str">
-        <v/>
-      </c>
-      <c r="K5" t="str">
-        <v/>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6">
-        <v>1</v>
-      </c>
-      <c r="B6" t="str">
-        <v>WANG,MEI(03/15/1960)</v>
-      </c>
-      <c r="C6" t="str">
-        <v>F</v>
-      </c>
-      <c r="D6" t="str">
-        <v>WC</v>
-      </c>
-      <c r="E6" t="str">
-        <v>SHOULDER</v>
-      </c>
-      <c r="F6" t="str">
-        <v>R</v>
-      </c>
-      <c r="G6" t="str">
-        <v>IE</v>
-      </c>
-      <c r="H6" t="str">
-        <v>M75.11,M25.511</v>
-      </c>
-      <c r="I6" t="str">
-        <v/>
-      </c>
-      <c r="J6" t="str">
-        <v>NECK</v>
-      </c>
-      <c r="K6" t="str">
-        <v>HTN,DM</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7">
-        <v>2</v>
-      </c>
-      <c r="B7" t="str">
-        <v>WANG,MEI(03/15/1960)</v>
-      </c>
-      <c r="C7" t="str">
-        <v>F</v>
-      </c>
-      <c r="D7" t="str">
-        <v>WC</v>
-      </c>
-      <c r="E7" t="str">
-        <v>SHOULDER</v>
-      </c>
-      <c r="F7" t="str">
-        <v>R</v>
-      </c>
-      <c r="G7" t="str">
-        <v>TX</v>
-      </c>
-      <c r="H7" t="str">
-        <v/>
-      </c>
-      <c r="I7" t="str">
-        <v/>
-      </c>
-      <c r="J7" t="str">
-        <v/>
-      </c>
-      <c r="K7" t="str">
-        <v/>
+      <c r="U4" t="str">
+        <v>Hypertension,Cholesterol</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:K7"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:U4"/>
   </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <cols>
-    <col min="1" max="1" width="16.83203125" customWidth="1"/>
-    <col min="2" max="2" width="10.83203125" customWidth="1"/>
+    <col min="1" max="1" width="20.83203125" customWidth="1"/>
+    <col min="2" max="2" width="28.83203125" customWidth="1"/>
     <col min="3" max="3" width="55.83203125" customWidth="1"/>
-    <col min="4" max="4" width="25.83203125" customWidth="1"/>
+    <col min="4" max="4" width="35.83203125" customWidth="1"/>
+    <col min="5" max="5" width="65.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -694,164 +720,370 @@
       <c r="D1" t="str">
         <v>Example</v>
       </c>
+      <c r="E1" t="str">
+        <v>Valid Values</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>DOS</v>
+        <v>Patient</v>
       </c>
       <c r="B2" t="str">
         <v>Yes</v>
       </c>
       <c r="C2" t="str">
-        <v>Visit number (1, 2, 3...)</v>
+        <v>Name and DOB: NAME(MM/DD/YYYY)</v>
       </c>
       <c r="D2" t="str">
-        <v>1</v>
+        <v>CHEN,AIJIN(09/27/1956)</v>
+      </c>
+      <c r="E2" t="str">
+        <v/>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>Patient</v>
+        <v>Gender</v>
       </c>
       <c r="B3" t="str">
         <v>Yes</v>
       </c>
       <c r="C3" t="str">
-        <v>Name and DOB: NAME(MM/DD/YYYY)</v>
+        <v>M or F</v>
       </c>
       <c r="D3" t="str">
-        <v>CHEN,AIJIN(09/27/1956)</v>
+        <v>F</v>
+      </c>
+      <c r="E3" t="str">
+        <v>M, F</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="str">
-        <v>Gender</v>
+        <v>Insurance</v>
       </c>
       <c r="B4" t="str">
         <v>Yes</v>
       </c>
       <c r="C4" t="str">
-        <v>M or F</v>
+        <v>Insurance type</v>
       </c>
       <c r="D4" t="str">
-        <v>F</v>
+        <v>HF</v>
+      </c>
+      <c r="E4" t="str">
+        <v>HF, OPTUM, WC, VC, ELDERPLAN, NONE</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="str">
-        <v>Insurance</v>
+        <v>BodyPart</v>
       </c>
       <c r="B5" t="str">
         <v>Yes</v>
       </c>
       <c r="C5" t="str">
-        <v>HF, OPTUM, WC, VC, ELDERPLAN, NONE</v>
+        <v>Primary body part</v>
       </c>
       <c r="D5" t="str">
-        <v>HF</v>
+        <v>LBP</v>
+      </c>
+      <c r="E5" t="str">
+        <v>LBP, NECK, SHOULDER, KNEE, ELBOW, HIP, MID_LOW_BACK, etc.</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="str">
-        <v>BodyPart</v>
+        <v>Laterality</v>
       </c>
       <c r="B6" t="str">
         <v>Yes</v>
       </c>
       <c r="C6" t="str">
-        <v>LBP, NECK, SHOULDER, KNEE, etc.</v>
+        <v>Side</v>
       </c>
       <c r="D6" t="str">
-        <v>LBP</v>
+        <v>B</v>
+      </c>
+      <c r="E6" t="str">
+        <v>B (bilateral), L (left), R (right)</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="str">
-        <v>Laterality</v>
+        <v>ICD</v>
       </c>
       <c r="B7" t="str">
         <v>Yes</v>
       </c>
       <c r="C7" t="str">
-        <v>B (bilateral), L (left), R (right)</v>
+        <v>Comma-separated ICD-10 codes</v>
       </c>
       <c r="D7" t="str">
-        <v>B</v>
+        <v>M54.50,M54.41</v>
+      </c>
+      <c r="E7" t="str">
+        <v/>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="str">
-        <v>NoteType</v>
+        <v>CPT</v>
       </c>
       <c r="B8" t="str">
-        <v>Yes</v>
+        <v>No</v>
       </c>
       <c r="C8" t="str">
-        <v>IE (Initial), TX (Treatment), RE (Re-eval)</v>
+        <v>Comma-separated CPT codes with units. Empty TX = auto-fill by insurance.</v>
       </c>
       <c r="D8" t="str">
-        <v>IE</v>
+        <v>97810,97811x3</v>
+      </c>
+      <c r="E8" t="str">
+        <v/>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="str">
-        <v>ICD</v>
+        <v>TotalVisits</v>
       </c>
       <c r="B9" t="str">
-        <v>IE only</v>
+        <v>Yes</v>
       </c>
       <c r="C9" t="str">
-        <v>Comma-separated ICD-10 codes. TX inherits from IE.</v>
+        <v>Total visits including IE. System generates 1 IE + (N-1) TX.</v>
       </c>
       <c r="D9" t="str">
-        <v>M54.50,M54.41</v>
+        <v>12</v>
+      </c>
+      <c r="E9" t="str">
+        <v>1-30</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="str">
-        <v>CPT</v>
+        <v>PainWorst</v>
       </c>
       <c r="B10" t="str">
-        <v>Optional</v>
+        <v>Default: 8</v>
       </c>
       <c r="C10" t="str">
-        <v>Comma-separated CPT codes with units. Empty TX = auto-fill.</v>
+        <v>Worst pain level (0-10)</v>
       </c>
       <c r="D10" t="str">
-        <v>97810,97811x3</v>
+        <v>8</v>
+      </c>
+      <c r="E10" t="str">
+        <v>0-10</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="str">
-        <v>SecondaryParts</v>
+        <v>PainBest</v>
       </c>
       <c r="B11" t="str">
-        <v>Optional</v>
+        <v>Default: 3</v>
       </c>
       <c r="C11" t="str">
-        <v>Comma-separated additional body parts</v>
+        <v>Best pain level (0-10)</v>
       </c>
       <c r="D11" t="str">
-        <v>NECK,SHOULDER</v>
+        <v>3</v>
+      </c>
+      <c r="E11" t="str">
+        <v>0-10</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="str">
+        <v>PainCurrent</v>
+      </c>
+      <c r="B12" t="str">
+        <v>Default: 6</v>
+      </c>
+      <c r="C12" t="str">
+        <v>Current pain level (0-10). Determines severity.</v>
+      </c>
+      <c r="D12" t="str">
+        <v>6</v>
+      </c>
+      <c r="E12" t="str">
+        <v>0-10</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="str">
+        <v>SymptomDuration</v>
+      </c>
+      <c r="B13" t="str">
+        <v>Default: 3 year(s)</v>
+      </c>
+      <c r="C13" t="str">
+        <v>How long symptoms have lasted</v>
+      </c>
+      <c r="D13" t="str">
+        <v>3 year(s)</v>
+      </c>
+      <c r="E13" t="str">
+        <v>N year(s), N month(s), N week(s), N day(s)</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="str">
+        <v>PainRadiation</v>
+      </c>
+      <c r="B14" t="str">
+        <v>Default: without radiation</v>
+      </c>
+      <c r="C14" t="str">
+        <v>Pain radiation description</v>
+      </c>
+      <c r="D14" t="str">
+        <v>without radiation</v>
+      </c>
+      <c r="E14" t="str">
+        <v>without radiation, with radiation to R arm, with radiation to L arm, with dizziness, etc.</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="str">
+        <v>PainTypes</v>
+      </c>
+      <c r="B15" t="str">
+        <v>Default: Dull,Aching</v>
+      </c>
+      <c r="C15" t="str">
+        <v>Comma-separated pain types</v>
+      </c>
+      <c r="D15" t="str">
+        <v>Dull,Aching</v>
+      </c>
+      <c r="E15" t="str">
+        <v>Dull, Burning, Freezing, Shooting, Tingling, Stabbing, Aching, Squeezing, Cramping</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="str">
+        <v>AssociatedSymptoms</v>
+      </c>
+      <c r="B16" t="str">
+        <v>Default: soreness</v>
+      </c>
+      <c r="C16" t="str">
+        <v>Comma-separated symptoms</v>
+      </c>
+      <c r="D16" t="str">
+        <v>soreness</v>
+      </c>
+      <c r="E16" t="str">
+        <v>soreness, stiffness, heaviness, weakness, numbness</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="str">
+        <v>CausativeFactors</v>
+      </c>
+      <c r="B17" t="str">
+        <v>Default: age related</v>
+      </c>
+      <c r="C17" t="str">
+        <v>Comma-separated causes</v>
+      </c>
+      <c r="D17" t="str">
+        <v>age related/degenerative changes</v>
+      </c>
+      <c r="E17" t="str">
+        <v>age related/degenerative changes, weather change, poor sleep, prolong walking, etc.</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="str">
+        <v>RelievingFactors</v>
+      </c>
+      <c r="B18" t="str">
+        <v>Default: Changing positions,Resting,Massage</v>
+      </c>
+      <c r="C18" t="str">
+        <v>Comma-separated relief methods</v>
+      </c>
+      <c r="D18" t="str">
+        <v>Changing positions,Resting</v>
+      </c>
+      <c r="E18" t="str">
+        <v>Moving around, Changing positions, Stretching, Resting, Lying down, Applying heating pad, Massage, Medications</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="str">
+        <v>SymptomScale</v>
+      </c>
+      <c r="B19" t="str">
+        <v>Default: 70%-80%</v>
+      </c>
+      <c r="C19" t="str">
+        <v>Symptom percentage scale</v>
+      </c>
+      <c r="D19" t="str">
+        <v>70%-80%</v>
+      </c>
+      <c r="E19" t="str">
+        <v>10%, 10%-20%, 20%, ... 100%</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="str">
+        <v>PainFrequency</v>
+      </c>
+      <c r="B20" t="str">
+        <v>Default: Constant</v>
+      </c>
+      <c r="C20" t="str">
+        <v>Pain frequency (shorthand)</v>
+      </c>
+      <c r="D20" t="str">
+        <v>Constant</v>
+      </c>
+      <c r="E20" t="str">
+        <v>Intermittent, Occasional, Frequent, Constant</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="str">
+        <v>SecondaryParts</v>
+      </c>
+      <c r="B21" t="str">
+        <v>No</v>
+      </c>
+      <c r="C21" t="str">
+        <v>Comma-separated additional body parts</v>
+      </c>
+      <c r="D21" t="str">
+        <v>NECK,SHOULDER</v>
+      </c>
+      <c r="E21" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="str">
         <v>History</v>
       </c>
-      <c r="B12" t="str">
-        <v>Optional</v>
-      </c>
-      <c r="C12" t="str">
+      <c r="B22" t="str">
+        <v>No</v>
+      </c>
+      <c r="C22" t="str">
         <v>Comma-separated medical history</v>
       </c>
-      <c r="D12" t="str">
-        <v>HTN,DM,Pacemaker</v>
+      <c r="D22" t="str">
+        <v>Hypertension,Diabetes</v>
+      </c>
+      <c r="E22" t="str">
+        <v>Hypertension, Diabetes, Heart Disease, Pacemaker, Osteoporosis, Joint Replacement, etc.</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:D12"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:E22"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
feat: web-based patient editor + JSON batch endpoint + template regenerator
- Add POST /api/batch/json endpoint for form-based patient submission
- Add Patient Editor UI with localStorage draft persistence in BatchView
- Tab switch between Patient Editor (default) and Excel Upload (backup)
- Regenerate batch-template.xlsx with Instructions sheet and SoapText field
- Add scripts/gen-template.ts for template generation

Generated with [AWS Code](https://claude.ai/code)
via [Happy](https://happy.engineering)

Co-Authored-By: Claude <noreply@anthropic.com>
Co-Authored-By: Happy <yesreply@happy.engineering>
</commit_message>
<xml_diff>
--- a/templates/batch-template.xlsx
+++ b/templates/batch-template.xlsx
@@ -5,6 +5,7 @@
   <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
   <sheets>
     <sheet sheetId="1" name="Patients" state="visible" r:id="rId4"/>
+    <sheet sheetId="2" name="Instructions" state="visible" r:id="rId5"/>
   </sheets>
   <calcPr calcId="171027"/>
 </workbook>
@@ -19,63 +20,154 @@
     <comment ref="A2" authorId="0">
       <text>
         <r>
-          <t>NAME(MM/DD/YYYY)</t>
+          <t>Format: LAST,FIRST(MM/DD/YYYY)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A3" authorId="0">
+      <text>
+        <r>
+          <t>M or F</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A4" authorId="0">
+      <text>
+        <r>
+          <t>HF | OPTUM | WC | VC | ELDERPLAN | NONE</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A5" authorId="0">
+      <text>
+        <r>
+          <t>LBP, NECK, UPPER_BACK, MIDDLE_BACK, MID_LOW_BACK, SHOULDER, ELBOW, WRIST, HAND, HIP, KNEE, ANKLE, FOOT</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A6" authorId="0">
+      <text>
+        <r>
+          <t>B (bilateral) | L (left) | R (right)</t>
         </r>
       </text>
     </comment>
     <comment ref="A7" authorId="0">
       <text>
         <r>
-          <t>Comma-separated, e.g. M54.50,M54.41</t>
+          <t>Comma-separated ICD-10 codes. Required for Full mode</t>
         </r>
       </text>
     </comment>
     <comment ref="A8" authorId="0">
       <text>
         <r>
-          <t>e.g. 97810,97811x3</t>
+          <t>Format: CODE or CODExUNITS. Auto-filled if empty</t>
         </r>
       </text>
     </comment>
     <comment ref="A9" authorId="0">
       <text>
         <r>
-          <t>1-30 (1 IE + N-1 TX)</t>
+          <t>Number of visits (IE + TX). Min 1</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A10" authorId="0">
+      <text>
+        <r>
+          <t>0-10 scale. Default: 7-8</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A11" authorId="0">
+      <text>
+        <r>
+          <t>0-10 scale. Default: 2-3</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A12" authorId="0">
+      <text>
+        <r>
+          <t>0-10 scale. Default: 5-7</t>
         </r>
       </text>
     </comment>
     <comment ref="A13" authorId="0">
       <text>
         <r>
-          <t>e.g. 3 year(s)</t>
+          <t>N year(s) | N month(s) | N week(s). Default: 3 year(s)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A14" authorId="0">
+      <text>
+        <r>
+          <t>Radiation description</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A15" authorId="0">
+      <text>
+        <r>
+          <t>Comma-separated: Dull, Aching, Stabbing, Sharp, Throbbing, Burning</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A16" authorId="0">
+      <text>
+        <r>
+          <t>Comma-separated: soreness, stiffness, numbness, tingling, weakness</t>
         </r>
       </text>
     </comment>
     <comment ref="A17" authorId="0">
       <text>
         <r>
-          <t>Comma-separated</t>
+          <t>Free text describing cause</t>
         </r>
       </text>
     </comment>
     <comment ref="A18" authorId="0">
       <text>
         <r>
-          <t>Comma-separated</t>
+          <t>Comma-separated relieving factors</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A19" authorId="0">
+      <text>
+        <r>
+          <t>Percentage range of symptom severity</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A20" authorId="0">
+      <text>
+        <r>
+          <t>INTERMITTENT | OCCASIONAL | FREQUENT | CONSTANT</t>
         </r>
       </text>
     </comment>
     <comment ref="A21" authorId="0">
       <text>
         <r>
-          <t>e.g. NECK,SHOULDER</t>
+          <t>Comma-separated secondary body parts</t>
         </r>
       </text>
     </comment>
     <comment ref="A22" authorId="0">
       <text>
         <r>
-          <t>e.g. Hypertension,Diabetes or N/A</t>
+          <t>Comma-separated medical history</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A23" authorId="0">
+      <text>
+        <r>
+          <t>Paste existing TX SOAP text here. Required for Continue mode</t>
         </r>
       </text>
     </comment>
@@ -84,7 +176,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="109">
   <si>
     <t>Field</t>
   </si>
@@ -134,6 +226,9 @@
     <t>F</t>
   </si>
   <si>
+    <t>M</t>
+  </si>
+  <si>
     <t>Insurance *</t>
   </si>
   <si>
@@ -176,18 +271,18 @@
     <t>97810,97811x3</t>
   </si>
   <si>
-    <t/>
-  </si>
-  <si>
     <t>TotalVisits *</t>
   </si>
   <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
     <t>PainWorst</t>
   </si>
   <si>
-    <t>8</t>
-  </si>
-  <si>
     <t>7</t>
   </si>
   <si>
@@ -294,13 +389,127 @@
   </si>
   <si>
     <t>Diabetes,Osteoporosis</t>
+  </si>
+  <si>
+    <t>SoapText</t>
+  </si>
+  <si>
+    <t>Required In</t>
+  </si>
+  <si>
+    <t>Format / Values</t>
+  </si>
+  <si>
+    <t>Example</t>
+  </si>
+  <si>
+    <t>All</t>
+  </si>
+  <si>
+    <t>Format: LAST,FIRST(MM/DD/YYYY)</t>
+  </si>
+  <si>
+    <t>M or F</t>
+  </si>
+  <si>
+    <t>HF | OPTUM | WC | VC | ELDERPLAN | NONE</t>
+  </si>
+  <si>
+    <t>Full/SOAP</t>
+  </si>
+  <si>
+    <t>LBP, NECK, UPPER_BACK, MIDDLE_BACK, MID_LOW_BACK, SHOULDER, ELBOW, WRIST, HAND, HIP, KNEE, ANKLE, FOOT</t>
+  </si>
+  <si>
+    <t>B (bilateral) | L (left) | R (right)</t>
+  </si>
+  <si>
+    <t>Full</t>
+  </si>
+  <si>
+    <t>Comma-separated ICD-10 codes. Required for Full mode</t>
+  </si>
+  <si>
+    <t>Format: CODE or CODExUNITS. Auto-filled if empty</t>
+  </si>
+  <si>
+    <t>Number of visits (IE + TX). Min 1</t>
+  </si>
+  <si>
+    <t>Optional</t>
+  </si>
+  <si>
+    <t>0-10 scale. Default: 7-8</t>
+  </si>
+  <si>
+    <t>0-10 scale. Default: 2-3</t>
+  </si>
+  <si>
+    <t>0-10 scale. Default: 5-7</t>
+  </si>
+  <si>
+    <t>N year(s) | N month(s) | N week(s). Default: 3 year(s)</t>
+  </si>
+  <si>
+    <t>Radiation description</t>
+  </si>
+  <si>
+    <t>Comma-separated: Dull, Aching, Stabbing, Sharp, Throbbing, Burning</t>
+  </si>
+  <si>
+    <t>Comma-separated: soreness, stiffness, numbness, tingling, weakness</t>
+  </si>
+  <si>
+    <t>Free text describing cause</t>
+  </si>
+  <si>
+    <t>Comma-separated relieving factors</t>
+  </si>
+  <si>
+    <t>Percentage range of symptom severity</t>
+  </si>
+  <si>
+    <t>INTERMITTENT | OCCASIONAL | FREQUENT | CONSTANT</t>
+  </si>
+  <si>
+    <t>Comma-separated secondary body parts</t>
+  </si>
+  <si>
+    <t>Comma-separated medical history</t>
+  </si>
+  <si>
+    <t>Continue</t>
+  </si>
+  <si>
+    <t>Paste existing TX SOAP text here. Required for Continue mode</t>
+  </si>
+  <si>
+    <t>—</t>
+  </si>
+  <si>
+    <t>Mode Guide</t>
+  </si>
+  <si>
+    <t>Full Batch</t>
+  </si>
+  <si>
+    <t>All * fields + ICD required. Generates SOAP + fills ICD/CPT + billing in MDLand.</t>
+  </si>
+  <si>
+    <t>SOAP Only</t>
+  </si>
+  <si>
+    <t>All * fields except ICD/CPT. Generates SOAP notes only, no MDLand automation.</t>
+  </si>
+  <si>
+    <t>Patient/Gender/Insurance/TotalVisits + SoapText required. Continues TX from existing SOAP.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <color theme="1"/>
       <family val="2"/>
@@ -311,11 +520,14 @@
     <font>
       <b/>
       <color rgb="FFFFFFFF"/>
-      <sz val="11"/>
     </font>
     <font>
       <b/>
-      <sz val="11"/>
+    </font>
+    <font/>
+    <font>
+      <b/>
+      <sz val="12"/>
     </font>
   </fonts>
   <fills count="4">
@@ -327,12 +539,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF4472C4"/>
+        <fgColor rgb="FF2D3748"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor rgb="FFF7FAFC"/>
       </patternFill>
     </fill>
   </fills>
@@ -348,11 +560,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -692,17 +909,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K22"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
-      <selection pane="bottomRight"/>
-    </sheetView>
-  </sheetViews>
+  <dimension ref="A1:K23"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="1" width="22" customWidth="1"/>
-    <col min="2" max="11" width="30" customWidth="1"/>
+    <col min="2" max="11" width="28" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
@@ -740,7 +951,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>11</v>
       </c>
@@ -751,7 +962,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>14</v>
       </c>
@@ -759,259 +970,599 @@
         <v>15</v>
       </c>
       <c r="C3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C4" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B5" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C5" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B6" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C6" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B7" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C7" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B8" t="s">
-        <v>29</v>
-      </c>
-      <c r="C8" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B9">
-        <v>12</v>
-      </c>
-      <c r="C9">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>32</v>
+      </c>
+      <c r="C9" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B10" t="s">
         <v>33</v>
       </c>
       <c r="C10" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B11" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C11" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B12" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C12" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B13" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C13" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B14" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C14" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B15" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C15" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B16" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C16" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B17" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C17" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B18" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C18" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B19" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C19" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B20" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C20" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="B21" t="s">
-        <v>30</v>
+        <v>66</v>
       </c>
       <c r="C21" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B22" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C22" t="s">
-        <v>69</v>
+        <v>70</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" s="3" t="s">
+        <v>71</v>
       </c>
     </row>
   </sheetData>
-  <dataValidations count="12">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" errorTitle="PainWorst" error="Valid: 10, 9, 8, 7, 6" sqref="B10:K10">
-      <formula1>"10,9,8,7,6,5,4,3,2,1,0"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" errorTitle="PainBest" error="Valid: 10, 9, 8, 7, 6" sqref="B11:K11">
-      <formula1>"10,9,8,7,6,5,4,3,2,1,0"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" errorTitle="PainCurrent" error="Valid: 10, 9, 8, 7, 6" sqref="B12:K12">
-      <formula1>"10,9,8,7,6,5,4,3,2,1,0"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" errorTitle="PainRadiation" error="Valid: without radiation, with radiation to R arm, with radiation to L arm, with radiation to R leg, with radiation to L leg" sqref="B14:K14">
-      <formula1>"without radiation,with radiation to R arm,with radiation to L arm,with radiation to R leg,with radiation to L leg,with radiation to bilateral legs"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" errorTitle="PainTypes" error="Valid: Dull,Aching, Dull,Stabbing, Aching,Stabbing, Dull, Aching" sqref="B15:K15">
-      <formula1>"Dull,Aching,Dull,Stabbing,Aching,Stabbing,Dull,Aching,Stabbing,Sharp,Burning,Throbbing"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" errorTitle="AssociatedSymptoms" error="Valid: soreness, tightness, stiffness, weakness, numbness" sqref="B16:K16">
-      <formula1>"soreness,tightness,stiffness,weakness,numbness,soreness,stiffness,tightness,weakness,stiffness,soreness"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" errorTitle="SymptomScale" error="Valid: 90%-100%, 80%-90%, 70%-80%, 60%-70%, 50%-60%" sqref="B19:K19">
-      <formula1>"90%-100%,80%-90%,70%-80%,60%-70%,50%-60%,40%-50%"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" errorTitle="PainFrequency" error="Valid: Constant, Frequent, Occasional, Intermittent" sqref="B20:K20">
-      <formula1>"Constant,Frequent,Occasional,Intermittent"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" errorTitle="Gender" error="Valid: M, F" sqref="B3:K3">
-      <formula1>"M,F"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" errorTitle="Insurance" error="Valid: HF, OPTUM, WC, VC, ELDERPLAN" sqref="B4:K4">
-      <formula1>"HF,OPTUM,WC,VC,ELDERPLAN,NONE"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" errorTitle="BodyPart" error="Valid: LBP, NECK, SHOULDER, KNEE, HIP" sqref="B5:K5">
-      <formula1>"LBP,NECK,SHOULDER,KNEE,HIP,ELBOW,UPPER_BACK,MIDDLE_BACK,MID_LOW_BACK,WRIST,HAND,ANKLE,FOOT,THIGH,CALF,ARM,FOREARM"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" errorTitle="Laterality" error="Valid: B, L, R" sqref="B6:K6">
-      <formula1>"B,L,R"</formula1>
-    </dataValidation>
-  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
   <legacyDrawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D29"/>
+  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
+  <cols>
+    <col min="1" max="1" width="22" customWidth="1"/>
+    <col min="2" max="2" width="16" customWidth="1"/>
+    <col min="3" max="3" width="60" customWidth="1"/>
+    <col min="4" max="4" width="30" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" t="s">
+        <v>75</v>
+      </c>
+      <c r="C2" t="s">
+        <v>76</v>
+      </c>
+      <c r="D2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" t="s">
+        <v>75</v>
+      </c>
+      <c r="C3" t="s">
+        <v>77</v>
+      </c>
+      <c r="D3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" t="s">
+        <v>75</v>
+      </c>
+      <c r="C4" t="s">
+        <v>78</v>
+      </c>
+      <c r="D4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5" t="s">
+        <v>79</v>
+      </c>
+      <c r="C5" t="s">
+        <v>80</v>
+      </c>
+      <c r="D5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6" t="s">
+        <v>79</v>
+      </c>
+      <c r="C6" t="s">
+        <v>81</v>
+      </c>
+      <c r="D6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B7" t="s">
+        <v>82</v>
+      </c>
+      <c r="C7" t="s">
+        <v>83</v>
+      </c>
+      <c r="D7" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>29</v>
+      </c>
+      <c r="B8" t="s">
+        <v>82</v>
+      </c>
+      <c r="C8" t="s">
+        <v>84</v>
+      </c>
+      <c r="D8" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B9" t="s">
+        <v>75</v>
+      </c>
+      <c r="C9" t="s">
+        <v>85</v>
+      </c>
+      <c r="D9" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>34</v>
+      </c>
+      <c r="B10" t="s">
+        <v>86</v>
+      </c>
+      <c r="C10" t="s">
+        <v>87</v>
+      </c>
+      <c r="D10" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>36</v>
+      </c>
+      <c r="B11" t="s">
+        <v>86</v>
+      </c>
+      <c r="C11" t="s">
+        <v>88</v>
+      </c>
+      <c r="D11" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>39</v>
+      </c>
+      <c r="B12" t="s">
+        <v>86</v>
+      </c>
+      <c r="C12" t="s">
+        <v>89</v>
+      </c>
+      <c r="D12" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>42</v>
+      </c>
+      <c r="B13" t="s">
+        <v>86</v>
+      </c>
+      <c r="C13" t="s">
+        <v>90</v>
+      </c>
+      <c r="D13" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>45</v>
+      </c>
+      <c r="B14" t="s">
+        <v>86</v>
+      </c>
+      <c r="C14" t="s">
+        <v>91</v>
+      </c>
+      <c r="D14" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>48</v>
+      </c>
+      <c r="B15" t="s">
+        <v>86</v>
+      </c>
+      <c r="C15" t="s">
+        <v>92</v>
+      </c>
+      <c r="D15" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>51</v>
+      </c>
+      <c r="B16" t="s">
+        <v>86</v>
+      </c>
+      <c r="C16" t="s">
+        <v>93</v>
+      </c>
+      <c r="D16" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>54</v>
+      </c>
+      <c r="B17" t="s">
+        <v>86</v>
+      </c>
+      <c r="C17" t="s">
+        <v>94</v>
+      </c>
+      <c r="D17" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>57</v>
+      </c>
+      <c r="B18" t="s">
+        <v>86</v>
+      </c>
+      <c r="C18" t="s">
+        <v>95</v>
+      </c>
+      <c r="D18" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>60</v>
+      </c>
+      <c r="B19" t="s">
+        <v>86</v>
+      </c>
+      <c r="C19" t="s">
+        <v>96</v>
+      </c>
+      <c r="D19" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>63</v>
+      </c>
+      <c r="B20" t="s">
+        <v>86</v>
+      </c>
+      <c r="C20" t="s">
+        <v>97</v>
+      </c>
+      <c r="D20" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>66</v>
+      </c>
+      <c r="B21" t="s">
+        <v>86</v>
+      </c>
+      <c r="C21" t="s">
+        <v>98</v>
+      </c>
+      <c r="D21" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>68</v>
+      </c>
+      <c r="B22" t="s">
+        <v>86</v>
+      </c>
+      <c r="C22" t="s">
+        <v>99</v>
+      </c>
+      <c r="D22" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>71</v>
+      </c>
+      <c r="B23" t="s">
+        <v>100</v>
+      </c>
+      <c r="C23" t="s">
+        <v>101</v>
+      </c>
+      <c r="D23" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A26" s="6" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="B27" t="s">
+        <v>105</v>
+      </c>
+      <c r="C27"/>
+      <c r="D27"/>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="B28" t="s">
+        <v>107</v>
+      </c>
+      <c r="C28"/>
+      <c r="D28"/>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="B29" t="s">
+        <v>108</v>
+      </c>
+      <c r="C29"/>
+      <c r="D29"/>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="B27:D27"/>
+    <mergeCell ref="B28:D28"/>
+    <mergeCell ref="B29:D29"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
+</worksheet>
 </file>
</xml_diff>